<commit_message>
Updated Standard Event Codes.
</commit_message>
<xml_diff>
--- a/Telemetry/Standard Event Codes.xlsx
+++ b/Telemetry/Standard Event Codes.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="215">
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Version 1.3</t>
+  </si>
   <si>
     <t>Category</t>
   </si>
@@ -88,6 +94,15 @@
     <t>ZONE:UNKNOWN_EVENT</t>
   </si>
   <si>
+    <t>ZONE:SAFEZONE:ENABLED</t>
+  </si>
+  <si>
+    <t>ZONE:SAFEZONE:DISABLED</t>
+  </si>
+  <si>
+    <t>ZONE:SAFEZONE:ALARM</t>
+  </si>
+  <si>
     <t>Idling</t>
   </si>
   <si>
@@ -202,6 +217,12 @@
     <t>BATTERY:DISCHARGING:INT</t>
   </si>
   <si>
+    <t>BATTERY:SHUNTING</t>
+  </si>
+  <si>
+    <t>DMT Only</t>
+  </si>
+  <si>
     <t>Accidents</t>
   </si>
   <si>
@@ -343,6 +364,66 @@
     <t>ALARM:HARDWARE:FAULT</t>
   </si>
   <si>
+    <t>ALARM:TAMPERING</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>BUTTON:ALARM:CLICK</t>
+  </si>
+  <si>
+    <t>Alarm button pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:ALARM:DOUBLE_CLICK</t>
+  </si>
+  <si>
+    <t>Alarm button double pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:ALARM:HOLD</t>
+  </si>
+  <si>
+    <t>Alarm button long pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:POWER:CLICK</t>
+  </si>
+  <si>
+    <t>Power button pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:POWER:DOUBLE_CLICK</t>
+  </si>
+  <si>
+    <t>Power button double clicked</t>
+  </si>
+  <si>
+    <t>BUTTON:POWER:HOLD</t>
+  </si>
+  <si>
+    <t>Power button long pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:x:CLICK</t>
+  </si>
+  <si>
+    <t>x = 1 to 3, i.e. Button 1, 2, or 3 pressed</t>
+  </si>
+  <si>
+    <t>BUTTON:x:DOUBLE_CLICK</t>
+  </si>
+  <si>
+    <t>x = 1 to 3, i.e. Button 1, 2, or 3 double clicked</t>
+  </si>
+  <si>
+    <t>BUTTON:x:HOLD</t>
+  </si>
+  <si>
+    <t>x = 1 to 3, i.e. Button 1, 2, or 3 long pressed</t>
+  </si>
+  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -566,24 +647,50 @@
   </si>
   <si>
     <t>MOVEMENT:DETECTED</t>
+  </si>
+  <si>
+    <t>MOVEMENT:UNAUTHORIZED</t>
+  </si>
+  <si>
+    <t>CalAmp Only</t>
+  </si>
+  <si>
+    <t>RECOVERY_MODE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -591,7 +698,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,6 +729,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -636,6 +749,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -648,8 +764,10 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -658,10 +776,7 @@
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -878,962 +993,954 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="30.0"/>
-    <col customWidth="1" min="3" max="3" width="46.86"/>
-    <col customWidth="1" min="4" max="4" width="19.57"/>
-    <col customWidth="1" min="5" max="5" width="24.29"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="29.5"/>
+    <col customWidth="1" min="3" max="3" width="41.0"/>
+    <col customWidth="1" min="4" max="4" width="17.13"/>
+    <col customWidth="1" min="5" max="5" width="21.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2">
+        <v>45252.0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12">
       <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="13">
       <c r="B13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="C13" s="9"/>
     </row>
     <row r="14">
       <c r="B14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>26</v>
+      <c r="C15" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="9" t="s">
+    <row r="18">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="9" t="s">
+    </row>
+    <row r="19">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="9" t="s">
+    <row r="20">
+      <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10" t="s">
+    </row>
+    <row r="21">
+      <c r="B21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="B22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="7" t="s">
+    </row>
+    <row r="23">
+      <c r="B23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="10"/>
-      <c r="B22" s="7" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="10"/>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="10"/>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="10"/>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="10" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10" t="s">
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B32" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="3"/>
-      <c r="B30" s="2" t="s">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4" t="s">
+      <c r="C33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="B34" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4" t="s">
+      <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7" t="s">
+      <c r="C35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="6"/>
+      <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
+      <c r="C36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4" t="s">
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="3"/>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="2" t="s">
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="3"/>
-      <c r="B40" s="2" t="s">
+      <c r="C41" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="3"/>
-      <c r="B41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="3"/>
-      <c r="B42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>66</v>
+      <c r="C42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3"/>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="2" t="s">
+    </row>
+    <row r="46">
+      <c r="A46" s="4"/>
+      <c r="B46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3"/>
-      <c r="B44" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D46" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="3"/>
-      <c r="B45" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="3"/>
-      <c r="B46" s="2" t="s">
+      <c r="D47" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="3"/>
-      <c r="B47" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="4"/>
-      <c r="B49" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="4"/>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="4"/>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="B53" s="11" t="s">
+      <c r="C53" s="4"/>
+      <c r="D53" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="3"/>
-      <c r="B56" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="2" t="s">
+    </row>
+    <row r="60">
+      <c r="B60" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D60" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9" t="s">
+      <c r="C61" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9" t="s">
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="4"/>
+      <c r="B62" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9" t="s">
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9" t="s">
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9" t="s">
+      <c r="B64" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9" t="s">
+      <c r="C64" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9" t="s">
-        <v>99</v>
-      </c>
+      <c r="D64" s="4"/>
     </row>
     <row r="65">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9" t="s">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66">
       <c r="A66" s="9"/>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C66" s="9"/>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2" t="s">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
+      <c r="C67" s="9"/>
+      <c r="D67" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="9"/>
+      <c r="D68" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="9"/>
       <c r="B70" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="9"/>
       <c r="B71" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>114</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C71" s="9"/>
       <c r="D71" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="9"/>
       <c r="B72" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="9" t="s">
+    </row>
+    <row r="74">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9" t="s">
+      <c r="B76" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="9" t="s">
+      <c r="D76" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="C77" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9" t="s">
+      <c r="D77" s="9"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="4" t="s">
+      <c r="C78" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C79" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D77" s="4"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="8"/>
-      <c r="B78" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
+      <c r="D79" s="9"/>
     </row>
     <row r="80">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" s="9"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4" t="s">
+      <c r="C81" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="D81" s="9"/>
     </row>
     <row r="82">
       <c r="A82" s="9"/>
       <c r="B82" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C82" s="9"/>
+      <c r="C82" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="D82" s="9"/>
     </row>
     <row r="83">
       <c r="A83" s="9"/>
       <c r="B83" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C83" s="9"/>
+        <v>133</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="D83" s="9"/>
     </row>
     <row r="84">
       <c r="A84" s="9"/>
       <c r="B84" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C84" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D84" s="9"/>
     </row>
     <row r="85">
       <c r="A85" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
+      <c r="D85" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="9"/>
       <c r="B86" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
+      <c r="D86" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="A87" s="9"/>
       <c r="B87" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
+        <v>140</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="9"/>
       <c r="B88" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
+        <v>142</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="9" t="s">
-        <v>140</v>
-      </c>
+      <c r="A89" s="9"/>
       <c r="B89" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D90" s="4"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="A91" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>146</v>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
+      <c r="D92" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" s="9"/>
-      <c r="B93" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
+      <c r="A93" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D93" s="5"/>
     </row>
     <row r="94">
-      <c r="A94" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D94" s="9"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D95" s="9"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
     </row>
     <row r="96">
-      <c r="A96" s="9" t="s">
-        <v>153</v>
-      </c>
+      <c r="A96" s="9"/>
       <c r="B96" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>155</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C96" s="9"/>
       <c r="D96" s="9"/>
     </row>
     <row r="97">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D97" s="9"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
     </row>
     <row r="98">
-      <c r="A98" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B98" s="12" t="s">
+      <c r="A98" s="9"/>
+      <c r="B98" s="9" t="s">
         <v>158</v>
       </c>
       <c r="C98" s="9"/>
@@ -1841,181 +1948,351 @@
     </row>
     <row r="99">
       <c r="A99" s="9"/>
-      <c r="B99" s="12" t="s">
+      <c r="B99" s="9" t="s">
         <v>159</v>
       </c>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
     </row>
     <row r="100">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="9"/>
+      <c r="B100" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="B101" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="B101" s="9" t="s">
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="9"/>
+      <c r="B102" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D101" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="B102" s="9" t="s">
+      <c r="B103" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C102" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="B103" s="9" t="s">
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="9"/>
+      <c r="B104" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D103" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="B104" s="9" t="s">
+      <c r="B105" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C104" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="B105" s="9" t="s">
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D105" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="B106" s="9" t="s">
+      <c r="C106" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D106" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="D106" s="5"/>
     </row>
     <row r="107">
-      <c r="B107" s="9" t="s">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D107" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="108">
       <c r="B108" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D108" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
     </row>
     <row r="109">
+      <c r="A109" s="9"/>
       <c r="B109" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D109" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110">
       <c r="B110" s="9" t="s">
         <v>176</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D110" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="D110" s="9"/>
     </row>
     <row r="111">
+      <c r="A111" s="9"/>
       <c r="B111" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D111" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="C111" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D111" s="9"/>
     </row>
     <row r="112">
+      <c r="A112" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="B112" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>9</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D112" s="9"/>
     </row>
     <row r="113">
+      <c r="A113" s="9"/>
       <c r="B113" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>9</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D113" s="9"/>
     </row>
     <row r="114">
-      <c r="B114" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="A114" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
     </row>
     <row r="115">
+      <c r="A115" s="9"/>
       <c r="B115" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>66</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
     </row>
     <row r="116">
+      <c r="A116" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="B116" s="9" t="s">
-        <v>183</v>
+        <v>188</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D117" s="12" t="s">
-        <v>99</v>
+        <v>190</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="6"/>
+      <c r="B135" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C135" s="6"/>
+      <c r="D135" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>